<commit_message>
add and update contents untill finish sixth practice exam
</commit_message>
<xml_diff>
--- a/simulated results.xlsx
+++ b/simulated results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Title</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>Udemy 6/6</t>
+  </si>
+  <si>
+    <t>AWS Certified Cloud Practitioner Exam (CLF-C01 - Portuguese) 20 questions</t>
+  </si>
+  <si>
+    <t>AWS Skill Builder</t>
   </si>
 </sst>
 </file>
@@ -69,13 +75,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="dd\-mmm"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +107,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -108,7 +128,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -124,9 +144,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -185,23 +205,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,42 +237,27 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,7 +272,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.4"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,181 +290,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,6 +548,48 @@
       <top/>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -575,39 +624,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -625,15 +641,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -647,7 +654,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -665,134 +672,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -821,6 +828,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
@@ -1160,13 +1173,13 @@
   <dimension ref="B1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="2" max="2" width="27.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="23.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="81" customWidth="1"/>
+    <col min="3" max="3" width="41.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="9.14285714285714" style="1"/>
     <col min="5" max="5" width="15.5714285714286" customWidth="1"/>
   </cols>
@@ -1305,7 +1318,12 @@
       <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="10"/>
+      <c r="D11" s="10">
+        <v>96</v>
+      </c>
+      <c r="E11" s="8">
+        <v>45103</v>
+      </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="6" t="s">
@@ -1314,105 +1332,120 @@
       <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="D12" s="11">
+        <v>67</v>
+      </c>
+      <c r="E12" s="8">
+        <v>45103</v>
+      </c>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="6"/>
-      <c r="E13" s="10"/>
+      <c r="B13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="10">
+        <v>90</v>
+      </c>
+      <c r="E13" s="8">
+        <v>45103</v>
+      </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="6"/>
-      <c r="E14" s="10"/>
+      <c r="E14" s="12"/>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="6"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="12"/>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="6"/>
-      <c r="E16" s="10"/>
+      <c r="E16" s="12"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="6"/>
-      <c r="E17" s="10"/>
+      <c r="E17" s="12"/>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="6"/>
-      <c r="E18" s="10"/>
+      <c r="E18" s="12"/>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="6"/>
-      <c r="E19" s="10"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="6"/>
-      <c r="E20" s="10"/>
+      <c r="E20" s="12"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="6"/>
-      <c r="E21" s="10"/>
+      <c r="E21" s="12"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="6"/>
-      <c r="E22" s="10"/>
+      <c r="E22" s="12"/>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="6"/>
-      <c r="E23" s="10"/>
+      <c r="E23" s="12"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="6"/>
-      <c r="E24" s="10"/>
+      <c r="E24" s="12"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="6"/>
-      <c r="E25" s="10"/>
+      <c r="E25" s="12"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="6"/>
-      <c r="E26" s="10"/>
+      <c r="E26" s="12"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="6"/>
-      <c r="E27" s="10"/>
+      <c r="E27" s="12"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="6"/>
-      <c r="E28" s="10"/>
+      <c r="E28" s="12"/>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="6"/>
-      <c r="E29" s="10"/>
+      <c r="E29" s="12"/>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="6"/>
-      <c r="E30" s="10"/>
+      <c r="E30" s="12"/>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="6"/>
-      <c r="E31" s="10"/>
+      <c r="E31" s="12"/>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="6"/>
-      <c r="E32" s="10"/>
+      <c r="E32" s="12"/>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="6"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="12"/>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="6"/>
-      <c r="E34" s="10"/>
+      <c r="E34" s="12"/>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="6"/>
-      <c r="E35" s="10"/>
+      <c r="E35" s="12"/>
     </row>
     <row r="36" ht="15.75" spans="2:5">
-      <c r="B36" s="11"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="14"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
chore: update content of  Others
</commit_message>
<xml_diff>
--- a/simulated results.xlsx
+++ b/simulated results.xlsx
@@ -117,11 +117,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -156,14 +156,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -178,7 +178,68 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -193,71 +254,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -326,181 +326,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -796,6 +796,45 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -811,45 +850,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -883,7 +883,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -904,61 +904,61 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -967,68 +967,68 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1076,12 +1076,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -1492,7 +1486,7 @@
   <dimension ref="B1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12:N12"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1543,12 +1537,12 @@
       <c r="H3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="26"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="24"/>
     </row>
     <row r="4" spans="2:14">
       <c r="B4" s="6" t="s">
@@ -1569,16 +1563,16 @@
       <c r="H4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="27">
+      <c r="I4" s="25">
         <v>50</v>
       </c>
-      <c r="J4" s="28">
+      <c r="J4" s="26">
         <v>87</v>
       </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="30"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="28"/>
     </row>
     <row r="5" spans="2:14">
       <c r="B5" s="6" t="s">
@@ -1599,16 +1593,16 @@
       <c r="H5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="29">
         <v>72</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="30">
         <v>95</v>
       </c>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="34"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="32"/>
     </row>
     <row r="6" spans="2:14">
       <c r="B6" s="6" t="s">
@@ -1629,16 +1623,16 @@
       <c r="H6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="35">
+      <c r="I6" s="33">
         <v>61</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J6" s="30">
         <v>83</v>
       </c>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="34"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="32"/>
     </row>
     <row r="7" spans="2:14">
       <c r="B7" s="6" t="s">
@@ -1659,16 +1653,16 @@
       <c r="H7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="35">
+      <c r="I7" s="33">
         <v>69</v>
       </c>
-      <c r="J7" s="32">
+      <c r="J7" s="30">
         <v>83</v>
       </c>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="34"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="32"/>
     </row>
     <row r="8" spans="2:14">
       <c r="B8" s="6" t="s">
@@ -1689,18 +1683,18 @@
       <c r="H8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="35">
+      <c r="I8" s="33">
         <v>69</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="30">
         <v>96</v>
       </c>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="34"/>
-    </row>
-    <row r="9" spans="2:14">
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="32"/>
+    </row>
+    <row r="9" ht="15.75" spans="2:14">
       <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
@@ -1719,16 +1713,16 @@
       <c r="H9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="36">
+      <c r="I9" s="34">
         <v>67</v>
       </c>
-      <c r="J9" s="37">
+      <c r="J9" s="35">
         <v>95</v>
       </c>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="39"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="37"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="6" t="s">
@@ -1783,12 +1777,12 @@
       <c r="H12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="26"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="24"/>
     </row>
     <row r="13" spans="2:14">
       <c r="B13" s="6" t="s">
@@ -1809,14 +1803,14 @@
       <c r="H13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="40">
+      <c r="I13" s="38">
         <v>84</v>
       </c>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="30"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="28"/>
     </row>
     <row r="14" spans="2:14">
       <c r="B14" s="6" t="s">
@@ -1837,14 +1831,14 @@
       <c r="H14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="41">
+      <c r="I14" s="39">
         <v>95</v>
       </c>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
-      <c r="N14" s="34"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="32"/>
     </row>
     <row r="15" spans="2:14">
       <c r="B15" s="6" t="s">
@@ -1865,14 +1859,14 @@
       <c r="H15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="41">
+      <c r="I15" s="39">
         <v>93</v>
       </c>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="34"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="32"/>
     </row>
     <row r="16" spans="2:14">
       <c r="B16" s="6" t="s">
@@ -1893,14 +1887,14 @@
       <c r="H16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="41">
+      <c r="I16" s="39">
         <v>84</v>
       </c>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="34"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="32"/>
     </row>
     <row r="17" spans="2:14">
       <c r="B17" s="6" t="s">
@@ -1921,14 +1915,14 @@
       <c r="H17" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="41">
+      <c r="I17" s="39">
         <v>80</v>
       </c>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="34"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="32"/>
     </row>
     <row r="18" ht="15.75" spans="2:14">
       <c r="B18" s="6" t="s">
@@ -1949,14 +1943,14 @@
       <c r="H18" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="42">
+      <c r="I18" s="40">
         <v>73</v>
       </c>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="39"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="37"/>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" s="6" t="s">
@@ -2002,47 +1996,47 @@
       <c r="D21" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="14">
         <v>95</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="8">
         <v>45120</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="44"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="41"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="42"/>
     </row>
     <row r="22" ht="15.75" spans="2:14">
       <c r="B22" s="6"/>
-      <c r="F22" s="18"/>
-      <c r="H22" s="19" t="s">
+      <c r="F22" s="16"/>
+      <c r="H22" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I22" s="45">
+      <c r="I22" s="43">
         <v>90</v>
       </c>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="44"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="42"/>
     </row>
     <row r="23" spans="2:14">
       <c r="B23" s="6"/>
       <c r="F23" s="8"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
     </row>
     <row r="24" spans="2:14">
       <c r="B24" s="6" t="s">
@@ -2054,14 +2048,14 @@
       <c r="D24" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="18"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="46"/>
-      <c r="K24" s="46"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46"/>
+      <c r="F24" s="16"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
     </row>
     <row r="25" spans="2:14">
       <c r="B25" s="6" t="s">
@@ -2073,79 +2067,79 @@
       <c r="D25" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="18"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
+      <c r="F25" s="16"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
     </row>
     <row r="26" spans="2:14">
       <c r="B26" s="6"/>
-      <c r="F26" s="18"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="46"/>
-      <c r="K26" s="46"/>
-      <c r="L26" s="46"/>
-      <c r="M26" s="46"/>
-      <c r="N26" s="46"/>
+      <c r="F26" s="16"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
     </row>
     <row r="27" spans="2:14">
       <c r="B27" s="6"/>
-      <c r="F27" s="18"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="46"/>
-      <c r="K27" s="46"/>
-      <c r="L27" s="46"/>
-      <c r="M27" s="46"/>
-      <c r="N27" s="46"/>
+      <c r="F27" s="16"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" s="6"/>
-      <c r="F28" s="18"/>
+      <c r="F28" s="16"/>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" s="6"/>
-      <c r="F29" s="18"/>
+      <c r="F29" s="16"/>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" s="6"/>
-      <c r="F30" s="18"/>
+      <c r="F30" s="16"/>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="6"/>
-      <c r="F31" s="18"/>
+      <c r="F31" s="16"/>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="6"/>
-      <c r="F32" s="18"/>
+      <c r="F32" s="16"/>
     </row>
     <row r="33" spans="2:6">
       <c r="B33" s="6"/>
-      <c r="F33" s="18"/>
+      <c r="F33" s="16"/>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" s="6"/>
-      <c r="F34" s="18"/>
+      <c r="F34" s="16"/>
     </row>
     <row r="35" spans="2:6">
       <c r="B35" s="6"/>
-      <c r="F35" s="18"/>
+      <c r="F35" s="16"/>
     </row>
     <row r="36" spans="2:6">
       <c r="B36" s="6"/>
-      <c r="F36" s="18"/>
+      <c r="F36" s="16"/>
     </row>
     <row r="37" ht="15.75" spans="2:6">
-      <c r="B37" s="21"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="24"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>